<commit_message>
Readme, License and Artifact Updates
</commit_message>
<xml_diff>
--- a/Artifacts/Digital Playbook Mapping.xlsx
+++ b/Artifacts/Digital Playbook Mapping.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -232,19 +232,67 @@
     <t>Research FDA and regulatory burden issues and drivers</t>
   </si>
   <si>
-    <t>Portia Scraping Results</t>
-  </si>
-  <si>
     <t>Scrape web data for correlating product label changes with adverse drug events using open source technology</t>
   </si>
   <si>
-    <t>Discovery and Requirements Analysis</t>
-  </si>
-  <si>
-    <t>Design Delivery</t>
-  </si>
-  <si>
     <t>Meet with user SMEs</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Discovery%20and%20Requirements%20Analysis.docx</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Design%20Delivery.docx</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Portia%20scraping%20results.JPG</t>
+  </si>
+  <si>
+    <t>Identified gaps in OpenFDA adverse drug event datasets</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/FAERS%20Variables%20ASCII%20Gaps.xls</t>
+  </si>
+  <si>
+    <t>Access OpenFDA API data through R interface</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Extracting%20FDA%20API%20data%20through%20R%20(Code).txt</t>
+  </si>
+  <si>
+    <t>Develop design prototype v1</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Design%20Prototype%20v1.twbx</t>
+  </si>
+  <si>
+    <t>Develop design prototype v2</t>
+  </si>
+  <si>
+    <t>Develop design prototype v3</t>
+  </si>
+  <si>
+    <t>Develop design prototype v4</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Design%20Prototype%20v2.twbx</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Design%20Prototype%20v3.twbx</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Design%20Prototype%20v4.twbx</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Event%20Count%20by%20Outcome%20Bar%20Chart.png</t>
+  </si>
+  <si>
+    <t>Develop correlation between drug combinations and adverse drug events</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Datasets/Drug.Combination.Percentage.combine.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/tree/master/Documents/Issues%20and%20Drivers</t>
   </si>
 </sst>
 </file>
@@ -254,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +314,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,10 +344,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -311,8 +368,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,10 +653,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +750,7 @@
       <c r="F2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>67</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -729,7 +788,7 @@
       <c r="F3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="9" t="s">
         <v>67</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -750,7 +809,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>42174</v>
+        <v>42173</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
@@ -758,25 +817,19 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="5" t="s">
         <v>61</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -803,12 +856,12 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>67</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -832,25 +885,28 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>42175</v>
+        <v>42174</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>61</v>
@@ -858,7 +914,7 @@
       <c r="J6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>61</v>
       </c>
       <c r="N6" s="5" t="s">
@@ -868,61 +924,452 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>42187</v>
+        <v>42174</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>42175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>42175</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>42175</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>42177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>42178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>42186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>42186</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>42187</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F15" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7" s="5" t="s">
+      <c r="G15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>42187</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T16" s="5" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U6">
-    <sortCondition ref="A2:A6"/>
+  <sortState ref="A2:T16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576 C2:C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Phases</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576 D2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Rituals</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E1048576 E2:E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>Artifacts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576 B2:B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Pools</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3:G5" r:id="rId2" display="https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Discovery%20and%20Requirements%20Analysis.docx"/>
+    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G10" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G14" r:id="rId10"/>
+    <hyperlink ref="G4" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1132,9 +1579,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1297,27 +1747,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDF1648-5EF8-4D8D-B906-BEFEFDAED3B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b91b61b-f977-492e-8765-13f1d3d131c0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a416958a-ab4e-452a-aea8-148780f674a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1342,9 +1780,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDF1648-5EF8-4D8D-B906-BEFEFDAED3B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4b91b61b-f977-492e-8765-13f1d3d131c0"/>
+    <ds:schemaRef ds:uri="a416958a-ab4e-452a-aea8-148780f674a9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Close to final updates
</commit_message>
<xml_diff>
--- a/Artifacts/Digital Playbook Mapping.xlsx
+++ b/Artifacts/Digital Playbook Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdamashek\SharePoint\ODEA - Documents\GSA 18F\Pool 1 docs\Artifacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdamashek\Documents\GitHub\OpenFDADesign\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -293,6 +293,21 @@
   </si>
   <si>
     <t>https://github.com/binarygroup/OpenFDADesign/tree/master/Documents/Issues%20and%20Drivers</t>
+  </si>
+  <si>
+    <t>Tested Design Prototype on several different mobile devices</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDADesign/blob/master/Artifacts/Mobile%20Accessibility%20Tests.docx</t>
+  </si>
+  <si>
+    <t>Met with user SME to review and get feedback on Design Prototype and usability</t>
+  </si>
+  <si>
+    <t>Produced a burndown chart for Pools 1 and 2 showing user story and issue resolution over time</t>
+  </si>
+  <si>
+    <t>Produced a GANTT chart for Pools 1 and 2 showing work over time</t>
   </si>
 </sst>
 </file>
@@ -653,10 +668,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,7 +989,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>42175</v>
       </c>
@@ -1012,7 +1027,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>42175</v>
       </c>
@@ -1258,7 +1273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>42187</v>
       </c>
@@ -1334,6 +1349,149 @@
         <v>61</v>
       </c>
       <c r="T16" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>42192</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>42192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>42192</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>42192</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1367,9 +1525,10 @@
     <hyperlink ref="G12" r:id="rId9"/>
     <hyperlink ref="G14" r:id="rId10"/>
     <hyperlink ref="G4" r:id="rId11"/>
+    <hyperlink ref="G17" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1579,12 +1738,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1747,15 +1903,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDF1648-5EF8-4D8D-B906-BEFEFDAED3B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4b91b61b-f977-492e-8765-13f1d3d131c0"/>
+    <ds:schemaRef ds:uri="a416958a-ab4e-452a-aea8-148780f674a9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1780,18 +1948,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDF1648-5EF8-4D8D-B906-BEFEFDAED3B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4b91b61b-f977-492e-8765-13f1d3d131c0"/>
-    <ds:schemaRef ds:uri="a416958a-ab4e-452a-aea8-148780f674a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>